<commit_message>
ford new model added
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rokib\classlearning1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFF685A-4A49-4B42-A1D0-E0121AD003CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198CCFDC-DAA1-4D2B-A8C3-81C2C04BB515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{9C96431A-75C3-4EBF-A9C5-B80A6578991B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C96431A-75C3-4EBF-A9C5-B80A6578991B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>ford</t>
   </si>
@@ -57,16 +57,26 @@
   </si>
   <si>
     <t>new model</t>
+  </si>
+  <si>
+    <t>new message added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583CC1F5-5D38-450E-990C-2694BC2DEF5C}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -441,7 +452,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -450,9 +461,26 @@
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>